<commit_message>
Updated AlgLIst with a minor addition
</commit_message>
<xml_diff>
--- a/SkienAlgsListFinal.xlsx
+++ b/SkienAlgsListFinal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://urfume-my.sharepoint.com/personal/sergey_osipov_urfu_me/Documents/AiSD2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1029" documentId="13_ncr:1_{BB64072A-02B6-4C3F-B1E2-71C6B558E3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3455C3C-B4C5-42F4-B17D-6059287B8E56}"/>
+  <xr:revisionPtr revIDLastSave="1034" documentId="13_ncr:1_{BB64072A-02B6-4C3F-B1E2-71C6B558E3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B64CAD8E-E30D-4049-8527-44BA8C8C3D54}"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="825" windowWidth="22200" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="1530" windowWidth="28050" windowHeight="14670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -1699,13 +1699,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5609EA63-45AF-4126-A392-111B73C106A8}" name="Таблица1" displayName="Таблица1" ref="A1:I107" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:I107" xr:uid="{5609EA63-45AF-4126-A392-111B73C106A8}">
-    <filterColumn colId="6">
-      <filters>
-        <dateGroupItem year="2025" month="12" dateTimeGrouping="month"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I107" xr:uid="{5609EA63-45AF-4126-A392-111B73C106A8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{93552DC0-400C-4041-9CCE-C18FD2B6831E}" name="Листинг" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{9E9E2B49-CA37-44D6-8AE2-28CC5F771432}" name="Имя" dataDxfId="6"/>
@@ -1922,10 +1916,10 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F70" sqref="F70"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1976,20 +1970,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="37">
         <v>26</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="37">
         <v>11</v>
       </c>
       <c r="F2" s="17" t="s">
@@ -2013,20 +2007,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="37">
         <v>67</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="37">
         <v>13</v>
       </c>
       <c r="F3" s="17" t="s">
@@ -2049,7 +2043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
         <v>18</v>
       </c>
@@ -2085,7 +2079,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -2113,7 +2107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
         <v>25</v>
       </c>
@@ -2149,7 +2143,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
         <v>28</v>
       </c>
@@ -2185,7 +2179,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>32</v>
       </c>
@@ -2221,7 +2215,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>37</v>
       </c>
@@ -2257,7 +2251,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>40</v>
       </c>
@@ -2293,7 +2287,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>44</v>
       </c>
@@ -2329,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>48</v>
       </c>
@@ -2365,7 +2359,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>52</v>
       </c>
@@ -2401,7 +2395,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>57</v>
       </c>
@@ -2437,7 +2431,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>62</v>
       </c>
@@ -2473,7 +2467,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>67</v>
       </c>
@@ -2509,7 +2503,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>70</v>
       </c>
@@ -2545,7 +2539,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="37" t="s">
         <v>70</v>
       </c>
@@ -2581,7 +2575,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>70</v>
       </c>
@@ -2617,7 +2611,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>82</v>
       </c>
@@ -2653,7 +2647,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>86</v>
       </c>
@@ -2689,7 +2683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>89</v>
       </c>
@@ -2725,7 +2719,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>92</v>
       </c>
@@ -2761,7 +2755,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>97</v>
       </c>
@@ -2797,7 +2791,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>102</v>
       </c>
@@ -2833,7 +2827,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>105</v>
       </c>
@@ -2869,7 +2863,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>108</v>
       </c>
@@ -2905,7 +2899,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>112</v>
       </c>
@@ -2941,7 +2935,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>115</v>
       </c>
@@ -2977,7 +2971,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>118</v>
       </c>
@@ -3013,7 +3007,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="37" t="s">
         <v>121</v>
       </c>
@@ -3049,7 +3043,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="37" t="s">
         <v>125</v>
       </c>
@@ -3085,7 +3079,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>128</v>
       </c>
@@ -3121,7 +3115,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>133</v>
       </c>
@@ -3157,7 +3151,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>136</v>
       </c>
@@ -3265,7 +3259,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>147</v>
       </c>
@@ -3301,7 +3295,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>151</v>
       </c>
@@ -3337,7 +3331,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>154</v>
       </c>
@@ -3373,7 +3367,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>157</v>
       </c>
@@ -3409,7 +3403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>157</v>
       </c>
@@ -3445,7 +3439,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>163</v>
       </c>
@@ -3481,7 +3475,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>165</v>
       </c>
@@ -3517,7 +3511,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>168</v>
       </c>
@@ -3553,7 +3547,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>171</v>
       </c>
@@ -3589,7 +3583,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>175</v>
       </c>
@@ -3625,7 +3619,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>179</v>
       </c>
@@ -3661,7 +3655,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>181</v>
       </c>
@@ -3697,7 +3691,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>184</v>
       </c>
@@ -3733,7 +3727,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>186</v>
       </c>
@@ -3762,7 +3756,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>189</v>
       </c>
@@ -3849,7 +3843,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>198</v>
       </c>
@@ -3878,7 +3872,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>201</v>
       </c>
@@ -3907,7 +3901,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>205</v>
       </c>
@@ -3936,7 +3930,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>208</v>
       </c>
@@ -3965,7 +3959,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>212</v>
       </c>
@@ -3994,7 +3988,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>215</v>
       </c>
@@ -4023,7 +4017,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>218</v>
       </c>
@@ -4052,7 +4046,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>222</v>
       </c>
@@ -4081,7 +4075,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>226</v>
       </c>
@@ -4110,7 +4104,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>230</v>
       </c>
@@ -4139,7 +4133,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>233</v>
       </c>
@@ -4168,7 +4162,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>236</v>
       </c>
@@ -4197,7 +4191,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>240</v>
       </c>
@@ -4226,7 +4220,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>243</v>
       </c>
@@ -4255,7 +4249,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>246</v>
       </c>
@@ -4313,7 +4307,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>253</v>
       </c>
@@ -4342,7 +4336,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>257</v>
       </c>
@@ -4458,7 +4452,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>270</v>
       </c>
@@ -4487,7 +4481,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>274</v>
       </c>
@@ -4516,7 +4510,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>277</v>
       </c>
@@ -4545,7 +4539,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>280</v>
       </c>
@@ -4574,7 +4568,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>284</v>
       </c>
@@ -4603,7 +4597,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>287</v>
       </c>
@@ -4632,7 +4626,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>290</v>
       </c>
@@ -4661,7 +4655,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>293</v>
       </c>
@@ -4690,7 +4684,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>296</v>
       </c>
@@ -4719,7 +4713,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>301</v>
       </c>
@@ -4777,7 +4771,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
         <v>307</v>
       </c>
@@ -4806,7 +4800,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
         <v>310</v>
       </c>
@@ -4835,7 +4829,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
         <v>313</v>
       </c>
@@ -4864,7 +4858,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>316</v>
       </c>
@@ -4893,7 +4887,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>320</v>
       </c>
@@ -4922,7 +4916,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>323</v>
       </c>
@@ -4951,7 +4945,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>327</v>
       </c>
@@ -4980,7 +4974,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>330</v>
       </c>
@@ -5038,7 +5032,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>336</v>
       </c>
@@ -5067,7 +5061,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>339</v>
       </c>
@@ -5096,7 +5090,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>343</v>
       </c>
@@ -5125,7 +5119,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>347</v>
       </c>
@@ -5154,7 +5148,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>350</v>
       </c>
@@ -5183,7 +5177,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>353</v>
       </c>
@@ -5212,7 +5206,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>356</v>
       </c>
@@ -5241,7 +5235,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>359</v>
       </c>
@@ -5270,7 +5264,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>362</v>
       </c>
@@ -5299,7 +5293,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>365</v>
       </c>
@@ -5328,7 +5322,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>368</v>
       </c>
@@ -5357,7 +5351,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>371</v>
       </c>

</xml_diff>